<commit_message>
fixxed the CRAN revision requests.
 * Make Description a paragraph (Done)
 * remove the lisence file and remove the line from the decription (done)
 * fix where the functions write by defalt. Make sure the user has to specify. (done)
 * Your examples are commented out. Please never do that.
Please wrap the examples in /donttest{}. (done)

updated R. Ran Recheck
</commit_message>
<xml_diff>
--- a/Notes/checklist.xlsx
+++ b/Notes/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billy\OneDrive\Documents\R\MobileTrigger\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DD2BB0-87A5-4DFB-AE9D-E634B1045617}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00B56BF-7D9A-4F68-957B-5172A48F9D6A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{09EAF802-D070-4406-8F34-0DAEB456642E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="26">
   <si>
     <t>Mobile Triggers Checklist</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Donttest</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41AF395-8AFA-4C37-BC67-0EF954FC2689}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -467,12 +473,12 @@
     <col min="3" max="3" width="27.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -488,8 +494,11 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -505,8 +514,11 @@
       <c r="E5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -522,8 +534,11 @@
       <c r="E6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -539,8 +554,11 @@
       <c r="E7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -556,8 +574,11 @@
       <c r="E8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -573,8 +594,11 @@
       <c r="E9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -590,8 +614,11 @@
       <c r="E10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -607,8 +634,11 @@
       <c r="E11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -624,8 +654,11 @@
       <c r="E12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -641,8 +674,11 @@
       <c r="E13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -658,8 +694,11 @@
       <c r="E14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>18</v>
       </c>

</xml_diff>